<commit_message>
Parsed .xlsx data successfully comitted to MSSQL Server
</commit_message>
<xml_diff>
--- a/ExcelReports/09-02-2014/Sales.xlsx
+++ b/ExcelReports/09-02-2014/Sales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>SaleId</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>StoreId</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +402,7 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +415,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -426,8 +432,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -440,8 +449,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -454,8 +466,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -468,8 +483,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -482,8 +500,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -496,8 +517,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -510,8 +534,11 @@
       <c r="D8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -524,8 +551,11 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -538,8 +568,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -550,6 +583,9 @@
         <v>9</v>
       </c>
       <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
         <v>10</v>
       </c>
     </row>

</xml_diff>